<commit_message>
implementado a geração de boleto para segunda via
</commit_message>
<xml_diff>
--- a/Api/documentos/templatesDocumentos/entrada.xlsx
+++ b/Api/documentos/templatesDocumentos/entrada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0103250\Desktop\teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0103250\Documents\Beneficios\Api\documentos\templatesDocumentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94476C1A-E735-478A-BDAF-9B49073C47E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80906D10-0534-49AB-9549-B5F639AFE814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30315" yWindow="750" windowWidth="19035" windowHeight="14625" xr2:uid="{62145E08-FC64-4926-9645-6421ABDCB8B5}"/>
+    <workbookView xWindow="3120" yWindow="900" windowWidth="21630" windowHeight="14625" xr2:uid="{62145E08-FC64-4926-9645-6421ABDCB8B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -410,8 +410,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,16 +438,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -451,6 +456,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,15 +495,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96065993-2972-4B1F-82A6-89F5DD33ED0F}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="160" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScale="160" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,27 +994,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
@@ -1024,12 +1031,12 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1048,38 +1055,38 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
@@ -1099,11 +1106,11 @@
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="2"/>
@@ -1112,11 +1119,11 @@
       <c r="A12" s="10"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="8"/>
@@ -1135,55 +1142,55 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="71"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="51" t="s">
+      <c r="B15" s="51"/>
+      <c r="C15" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="52"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F15" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="55">
+      <c r="G15" s="47"/>
+      <c r="H15" s="56">
         <v>37426</v>
       </c>
-      <c r="I15" s="56"/>
+      <c r="I15" s="57"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="53" t="s">
+      <c r="B16" s="55"/>
+      <c r="C16" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="54"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="11">
         <v>2021</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="44"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
@@ -1197,36 +1204,36 @@
       <c r="G17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="50"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="74"/>
     </row>
     <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
     </row>
     <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
@@ -1278,10 +1285,10 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="58"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="3"/>
@@ -1324,11 +1331,11 @@
       <c r="A28" s="18"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="19"/>
@@ -1348,11 +1355,11 @@
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="2"/>
@@ -1361,11 +1368,11 @@
       <c r="A31" s="10"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="8"/>
@@ -1384,55 +1391,55 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="51" t="s">
+      <c r="B34" s="51"/>
+      <c r="C34" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="52"/>
+      <c r="D34" s="51"/>
       <c r="E34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="45" t="s">
+      <c r="F34" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="46"/>
-      <c r="H34" s="55">
+      <c r="G34" s="47"/>
+      <c r="H34" s="56">
         <v>37426</v>
       </c>
-      <c r="I34" s="56"/>
+      <c r="I34" s="57"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="48"/>
-      <c r="C35" s="53" t="s">
+      <c r="B35" s="55"/>
+      <c r="C35" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="54"/>
+      <c r="D35" s="55"/>
       <c r="E35" s="11">
         <v>2021</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="44"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="45"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
@@ -1446,36 +1453,36 @@
       <c r="G36" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="49"/>
-      <c r="I36" s="50"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="53"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="41"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="74"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="39"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="50"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="49"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
@@ -1527,12 +1534,12 @@
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
       <c r="G42" s="3"/>

</xml_diff>

<commit_message>
atualização em larga escala no projeto
</commit_message>
<xml_diff>
--- a/Api/documentos/templatesDocumentos/entrada.xlsx
+++ b/Api/documentos/templatesDocumentos/entrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0103250\Documents\Beneficios\Api\documentos\templatesDocumentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80906D10-0534-49AB-9549-B5F639AFE814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E4AC1B-9D27-482D-888C-39C7FEB6ED5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="900" windowWidth="21630" windowHeight="14625" xr2:uid="{62145E08-FC64-4926-9645-6421ABDCB8B5}"/>
+    <workbookView xWindow="30360" yWindow="1605" windowWidth="21630" windowHeight="14625" xr2:uid="{62145E08-FC64-4926-9645-6421ABDCB8B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -387,27 +387,65 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -416,87 +454,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,15 +627,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>313592</xdr:colOff>
+      <xdr:colOff>295732</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>159727</xdr:rowOff>
+      <xdr:rowOff>82336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>417343</xdr:colOff>
+      <xdr:colOff>399483</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>167348</xdr:rowOff>
+      <xdr:rowOff>89957</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -664,8 +664,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="313592" y="5251939"/>
-          <a:ext cx="792482" cy="579121"/>
+          <a:off x="295732" y="5166305"/>
+          <a:ext cx="788360" cy="579121"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -976,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96065993-2972-4B1F-82A6-89F5DD33ED0F}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScale="160" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScale="160" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
@@ -994,27 +994,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="65"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
@@ -1031,12 +1031,12 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1055,38 +1055,38 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="71"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
@@ -1106,11 +1106,11 @@
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="2"/>
@@ -1119,11 +1119,11 @@
       <c r="A12" s="10"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="8"/>
@@ -1142,54 +1142,54 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="60"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="50" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="56">
+      <c r="G15" s="68"/>
+      <c r="H15" s="42">
         <v>37426</v>
       </c>
-      <c r="I15" s="57"/>
+      <c r="I15" s="43"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="54" t="s">
+      <c r="B16" s="66"/>
+      <c r="C16" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="66"/>
       <c r="E16" s="11">
         <v>2021</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="43"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1204,36 +1204,36 @@
       <c r="G17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="52"/>
-      <c r="I17" s="53"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="47"/>
     </row>
     <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="73"/>
-      <c r="I18" s="74"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
     </row>
     <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
     </row>
     <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
@@ -1249,8 +1249,8 @@
       <c r="G20" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
     </row>
     <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -1266,8 +1266,8 @@
       <c r="G21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="55"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -1285,10 +1285,10 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="3"/>
@@ -1296,23 +1296,23 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="10"/>
       <c r="H24" s="7"/>
       <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="23"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
@@ -1331,11 +1331,11 @@
       <c r="A28" s="18"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="19"/>
@@ -1355,11 +1355,11 @@
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="2"/>
@@ -1368,11 +1368,11 @@
       <c r="A31" s="10"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="8"/>
@@ -1391,54 +1391,54 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
       <c r="I33" s="45"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="50" t="s">
+      <c r="B34" s="64"/>
+      <c r="C34" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="51"/>
+      <c r="D34" s="64"/>
       <c r="E34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="56">
+      <c r="G34" s="68"/>
+      <c r="H34" s="42">
         <v>37426</v>
       </c>
-      <c r="I34" s="57"/>
+      <c r="I34" s="43"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="54" t="s">
+      <c r="B35" s="66"/>
+      <c r="C35" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="55"/>
+      <c r="D35" s="66"/>
       <c r="E35" s="11">
         <v>2021</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="43"/>
+      <c r="H35" s="44"/>
       <c r="I35" s="45"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1453,93 +1453,93 @@
       <c r="G36" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="52"/>
-      <c r="I36" s="53"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="47"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="42"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="73"/>
-      <c r="I37" s="74"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="49"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="42"/>
+      <c r="A38" s="56"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="48"/>
-      <c r="I38" s="49"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="51"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="30">
+      <c r="B39" s="70">
         <v>331</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="71"/>
       <c r="G39" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="33"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="53"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="71"/>
       <c r="G40" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H40" s="34"/>
-      <c r="I40" s="35"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="55"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="71"/>
       <c r="G41" s="4"/>
       <c r="H41" s="5"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
       <c r="G42" s="3"/>
@@ -1547,50 +1547,50 @@
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="29"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="41"/>
       <c r="G43" s="10"/>
       <c r="H43" s="7"/>
       <c r="I43" s="8"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H44" s="23" t="s">
+      <c r="H44" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="23"/>
+      <c r="I44" s="59"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25" t="s">
+      <c r="B45" s="73"/>
+      <c r="C45" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25" t="s">
+      <c r="D45" s="73"/>
+      <c r="E45" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26" t="s">
+      <c r="F45" s="73"/>
+      <c r="G45" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="H45" s="26"/>
+      <c r="H45" s="74"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
+      <c r="B47" s="72"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="21"/>
@@ -1598,30 +1598,19 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A6:I7"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="H15:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="A18:F19"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="A37:F38"/>
@@ -1635,19 +1624,30 @@
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="H34:I35"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="H15:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="A18:F19"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A6:I7"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>